<commit_message>
Advance in Excel Reader service advanced XLWorkbook class created
</commit_message>
<xml_diff>
--- a/FilesOrganizerIDOffice/src/main/resources/una/filesorganizeridoffice/xlsx/Formato Individual Funcionarios.xlsx
+++ b/FilesOrganizerIDOffice/src/main/resources/una/filesorganizeridoffice/xlsx/Formato Individual Funcionarios.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\N00148095\Desktop\Git\FileOrganizator\FilesOrganizatorIDOffice\src\main\resources\una\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\N00148095\Desktop\Git\FileOrganizer\FilesOrganizerIDOffice\src\main\resources\una\filesorganizeridoffice\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28BEB420-26BB-434E-9FD1-A8350C1C8B09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E431C3-A41A-41D0-BCEB-10B11EFA6F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{6C841B7B-D229-4537-91E2-FEAD6CCCD805}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="16200" xr2:uid="{6C841B7B-D229-4537-91E2-FEAD6CCCD805}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t xml:space="preserve">Nombre </t>
   </si>
@@ -87,9 +87,6 @@
   </si>
   <si>
     <t>Fecha de ingreso empresa</t>
-  </si>
-  <si>
-    <t>Identificacion</t>
   </si>
 </sst>
 </file>
@@ -135,16 +132,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -152,7 +149,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -160,6 +157,7 @@
     <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6272DC6E-8DC1-4A5D-8A06-05C5506732EA}">
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,8 +552,28 @@
         <v>16</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>17</v>
-      </c>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>

<commit_message>
Excel now is being read row by row and serializad into models with an own XL API
</commit_message>
<xml_diff>
--- a/FilesOrganizerIDOffice/src/main/resources/una/filesorganizeridoffice/xlsx/Formato Individual Funcionarios.xlsx
+++ b/FilesOrganizerIDOffice/src/main/resources/una/filesorganizeridoffice/xlsx/Formato Individual Funcionarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\N00148095\Desktop\Git\FileOrganizer\FilesOrganizerIDOffice\src\main\resources\una\filesorganizeridoffice\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\FileOrganizer\FilesOrganizerIDOffice\src\main\resources\una\filesorganizeridoffice\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E431C3-A41A-41D0-BCEB-10B11EFA6F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC007C1-DFDC-458F-ACC6-9DB8FF6E1F6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="16200" xr2:uid="{6C841B7B-D229-4537-91E2-FEAD6CCCD805}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{6C841B7B-D229-4537-91E2-FEAD6CCCD805}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -176,7 +176,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -474,11 +474,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6272DC6E-8DC1-4A5D-8A06-05C5506732EA}">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="10" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Adding support for employees to serializer
</commit_message>
<xml_diff>
--- a/FilesOrganizerIDOffice/src/main/resources/una/filesorganizeridoffice/xlsx/Formato Individual Funcionarios.xlsx
+++ b/FilesOrganizerIDOffice/src/main/resources/una/filesorganizeridoffice/xlsx/Formato Individual Funcionarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\FileOrganizer\FilesOrganizerIDOffice\src\main\resources\una\filesorganizeridoffice\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC007C1-DFDC-458F-ACC6-9DB8FF6E1F6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{643BAA1A-E260-4E02-BEF3-2513AE2B2852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{6C841B7B-D229-4537-91E2-FEAD6CCCD805}"/>
+    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11835" xr2:uid="{6C841B7B-D229-4537-91E2-FEAD6CCCD805}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -80,13 +80,13 @@
     <t>Oficina</t>
   </si>
   <si>
-    <t>Salario Bruto</t>
-  </si>
-  <si>
-    <t>Salario Neto</t>
-  </si>
-  <si>
     <t>Fecha de ingreso empresa</t>
+  </si>
+  <si>
+    <t>Salario Promedio</t>
+  </si>
+  <si>
+    <t>Tiene cuenta</t>
   </si>
 </sst>
 </file>
@@ -122,7 +122,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -145,11 +145,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -158,6 +169,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6272DC6E-8DC1-4A5D-8A06-05C5506732EA}">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,10 +507,10 @@
     <col min="12" max="12" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -543,16 +557,16 @@
         <v>13</v>
       </c>
       <c r="O1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="R1" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>